<commit_message>
small change in photography results file
</commit_message>
<xml_diff>
--- a/mutation-analysis/mutants-rasa/results_photography.xlsx
+++ b/mutation-analysis/mutants-rasa/results_photography.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\satori\user-simulator-evaluation\mutation-analysis\mutants-rasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772E6386-ED8C-4095-B4BE-C905D2B06671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6DE099-0A8C-4D5A-8C58-A029D0AC9E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="263">
   <si>
     <t>Sensei chat</t>
   </si>
@@ -177,6 +178,654 @@
   </si>
   <si>
     <t>SENSEI Mut. Score</t>
+  </si>
+  <si>
+    <t>mutant_CRE_002</t>
+  </si>
+  <si>
+    <t>mutant_CRE_003</t>
+  </si>
+  <si>
+    <t>mutant_CRE_004</t>
+  </si>
+  <si>
+    <t>mutant_CRE_007</t>
+  </si>
+  <si>
+    <t>mutant_CRE_009</t>
+  </si>
+  <si>
+    <t>mutant_CRE_011</t>
+  </si>
+  <si>
+    <t>mutant_CRE_012</t>
+  </si>
+  <si>
+    <t>mutant_CRE_013</t>
+  </si>
+  <si>
+    <t>mutant_CRE_014</t>
+  </si>
+  <si>
+    <t>mutant_CRE_015</t>
+  </si>
+  <si>
+    <t>mutant_CRE_016</t>
+  </si>
+  <si>
+    <t>mutant_DA_002</t>
+  </si>
+  <si>
+    <t>mutant_DA_004</t>
+  </si>
+  <si>
+    <t>mutant_DA_005</t>
+  </si>
+  <si>
+    <t>mutant_DA_007</t>
+  </si>
+  <si>
+    <t>mutant_DA_008</t>
+  </si>
+  <si>
+    <t>mutant_DA_010</t>
+  </si>
+  <si>
+    <t>mutant_DA_011</t>
+  </si>
+  <si>
+    <t>mutant_DA_013</t>
+  </si>
+  <si>
+    <t>mutant_DCS_002</t>
+  </si>
+  <si>
+    <t>mutant_DCS_003</t>
+  </si>
+  <si>
+    <t>mutant_DCS_004</t>
+  </si>
+  <si>
+    <t>mutant_DCS_007</t>
+  </si>
+  <si>
+    <t>mutant_DIP_002</t>
+  </si>
+  <si>
+    <t>mutant_DIP_006</t>
+  </si>
+  <si>
+    <t>mutant_DSYN_005</t>
+  </si>
+  <si>
+    <t>mutant_K2TP_003</t>
+  </si>
+  <si>
+    <t>mutant_K2TP_005</t>
+  </si>
+  <si>
+    <t>mutant_K2TP_008</t>
+  </si>
+  <si>
+    <t>mutant_K2TP_009</t>
+  </si>
+  <si>
+    <t>mutant_SO_001</t>
+  </si>
+  <si>
+    <t>mutant_SO_002</t>
+  </si>
+  <si>
+    <t>mutant_SO_003</t>
+  </si>
+  <si>
+    <t>mutant_SO_004</t>
+  </si>
+  <si>
+    <t>mutant_SO_005</t>
+  </si>
+  <si>
+    <t>mutant_SO_006</t>
+  </si>
+  <si>
+    <t>mutant_SO_007</t>
+  </si>
+  <si>
+    <t>mutant_SO_008</t>
+  </si>
+  <si>
+    <t>mutant_SO_009</t>
+  </si>
+  <si>
+    <t>mutant_SO_010</t>
+  </si>
+  <si>
+    <t>mutant_SO_011</t>
+  </si>
+  <si>
+    <t>mutant_SO_012</t>
+  </si>
+  <si>
+    <t>mutant_SO_013</t>
+  </si>
+  <si>
+    <t>mutant_SO_014</t>
+  </si>
+  <si>
+    <t>mutant_SO_015</t>
+  </si>
+  <si>
+    <t>mutant_SO_016</t>
+  </si>
+  <si>
+    <t>mutant_SO_017</t>
+  </si>
+  <si>
+    <t>mutant_SO_018</t>
+  </si>
+  <si>
+    <t>mutant_SO_019</t>
+  </si>
+  <si>
+    <t>mutant_SO_020</t>
+  </si>
+  <si>
+    <t>mutant_SO_021</t>
+  </si>
+  <si>
+    <t>mutant_SO_022</t>
+  </si>
+  <si>
+    <t>mutant_SO_023</t>
+  </si>
+  <si>
+    <t>mutant_SO_024</t>
+  </si>
+  <si>
+    <t>mutant_SO_025</t>
+  </si>
+  <si>
+    <t>mutant_SO_026</t>
+  </si>
+  <si>
+    <t>mutant_SO_027</t>
+  </si>
+  <si>
+    <t>mutant_SO_028</t>
+  </si>
+  <si>
+    <t>mutant_SO_029</t>
+  </si>
+  <si>
+    <t>mutant_SO_031</t>
+  </si>
+  <si>
+    <t>mutant_SO_032</t>
+  </si>
+  <si>
+    <t>mutant_SO_033</t>
+  </si>
+  <si>
+    <t>mutant_SO_034</t>
+  </si>
+  <si>
+    <t>mutant_SO_035</t>
+  </si>
+  <si>
+    <t>mutant_SO_036</t>
+  </si>
+  <si>
+    <t>mutant_SO_037</t>
+  </si>
+  <si>
+    <t>mutant_SO_038</t>
+  </si>
+  <si>
+    <t>mutant_SO_039</t>
+  </si>
+  <si>
+    <t>mutant_SO_040</t>
+  </si>
+  <si>
+    <t>mutant_SO_041</t>
+  </si>
+  <si>
+    <t>mutant_SO_043</t>
+  </si>
+  <si>
+    <t>mutant_SO_044</t>
+  </si>
+  <si>
+    <t>mutant_SO_045</t>
+  </si>
+  <si>
+    <t>mutant_SO_046</t>
+  </si>
+  <si>
+    <t>mutant_SO_047</t>
+  </si>
+  <si>
+    <t>mutant_SO_048</t>
+  </si>
+  <si>
+    <t>mutant_SO_049</t>
+  </si>
+  <si>
+    <t>mutant_SO_050</t>
+  </si>
+  <si>
+    <t>mutant_SO_051</t>
+  </si>
+  <si>
+    <t>mutant_SO_052</t>
+  </si>
+  <si>
+    <t>mutant_SO_053</t>
+  </si>
+  <si>
+    <t>mutant_SO_054</t>
+  </si>
+  <si>
+    <t>mutant_SO_055</t>
+  </si>
+  <si>
+    <t>mutant_SO_056</t>
+  </si>
+  <si>
+    <t>mutant_SO_057</t>
+  </si>
+  <si>
+    <t>mutant_SO_058</t>
+  </si>
+  <si>
+    <t>mutant_SO_059</t>
+  </si>
+  <si>
+    <t>mutant_SO_060</t>
+  </si>
+  <si>
+    <t>mutant_SO_061</t>
+  </si>
+  <si>
+    <t>mutant_SO_062</t>
+  </si>
+  <si>
+    <t>mutant_SO_063</t>
+  </si>
+  <si>
+    <t>mutant_SO_064</t>
+  </si>
+  <si>
+    <t>mutant_SO_065</t>
+  </si>
+  <si>
+    <t>mutant_SO_066</t>
+  </si>
+  <si>
+    <t>mutant_SO_067</t>
+  </si>
+  <si>
+    <t>mutant_SO_068</t>
+  </si>
+  <si>
+    <t>mutant_SO_069</t>
+  </si>
+  <si>
+    <t>mutant_SO_070</t>
+  </si>
+  <si>
+    <t>mutant_SO_071</t>
+  </si>
+  <si>
+    <t>mutant_SO_072</t>
+  </si>
+  <si>
+    <t>mutant_SO_073</t>
+  </si>
+  <si>
+    <t>mutant_SO_074</t>
+  </si>
+  <si>
+    <t>mutant_SO_075</t>
+  </si>
+  <si>
+    <t>mutant_SO_076</t>
+  </si>
+  <si>
+    <t>mutant_SO_077</t>
+  </si>
+  <si>
+    <t>mutant_SO_078</t>
+  </si>
+  <si>
+    <t>mutant_SO_079</t>
+  </si>
+  <si>
+    <t>mutant_SO_080</t>
+  </si>
+  <si>
+    <t>mutant_SO_081</t>
+  </si>
+  <si>
+    <t>mutant_SO_082</t>
+  </si>
+  <si>
+    <t>mutant_SO_083</t>
+  </si>
+  <si>
+    <t>mutant_SO_084</t>
+  </si>
+  <si>
+    <t>mutant_SO_085</t>
+  </si>
+  <si>
+    <t>mutant_SO_086</t>
+  </si>
+  <si>
+    <t>mutant_SO_087</t>
+  </si>
+  <si>
+    <t>mutant_SO_088</t>
+  </si>
+  <si>
+    <t>mutant_SO_089</t>
+  </si>
+  <si>
+    <t>mutant_SO_090</t>
+  </si>
+  <si>
+    <t>mutant_SO_091</t>
+  </si>
+  <si>
+    <t>mutant_SO_092</t>
+  </si>
+  <si>
+    <t>mutant_SO_093</t>
+  </si>
+  <si>
+    <t>mutant_SO_094</t>
+  </si>
+  <si>
+    <t>mutant_SO_095</t>
+  </si>
+  <si>
+    <t>mutant_SO_096</t>
+  </si>
+  <si>
+    <t>mutant_SO_097</t>
+  </si>
+  <si>
+    <t>mutant_SO_098</t>
+  </si>
+  <si>
+    <t>mutant_SO_099</t>
+  </si>
+  <si>
+    <t>mutant_SO_100</t>
+  </si>
+  <si>
+    <t>mutant_SO_101</t>
+  </si>
+  <si>
+    <t>mutant_SO_102</t>
+  </si>
+  <si>
+    <t>mutant_SO_103</t>
+  </si>
+  <si>
+    <t>mutant_SO_104</t>
+  </si>
+  <si>
+    <t>mutant_SO_105</t>
+  </si>
+  <si>
+    <t>mutant_SO_106</t>
+  </si>
+  <si>
+    <t>mutant_SO_107</t>
+  </si>
+  <si>
+    <t>mutant_SO_108</t>
+  </si>
+  <si>
+    <t>mutant_SO_109</t>
+  </si>
+  <si>
+    <t>mutant_SO_110</t>
+  </si>
+  <si>
+    <t>mutant_SO_112</t>
+  </si>
+  <si>
+    <t>mutant_SO_113</t>
+  </si>
+  <si>
+    <t>mutant_SO_114</t>
+  </si>
+  <si>
+    <t>mutant_SO_115</t>
+  </si>
+  <si>
+    <t>mutant_SO_117</t>
+  </si>
+  <si>
+    <t>mutant_SO_118</t>
+  </si>
+  <si>
+    <t>mutant_SO_119</t>
+  </si>
+  <si>
+    <t>mutant_SO_120</t>
+  </si>
+  <si>
+    <t>mutant_SO_121</t>
+  </si>
+  <si>
+    <t>mutant_SO_122</t>
+  </si>
+  <si>
+    <t>mutant_SO_123</t>
+  </si>
+  <si>
+    <t>mutant_SO_124</t>
+  </si>
+  <si>
+    <t>mutant_SO_125</t>
+  </si>
+  <si>
+    <t>mutant_SO_126</t>
+  </si>
+  <si>
+    <t>mutant_SO_127</t>
+  </si>
+  <si>
+    <t>mutant_SO_128</t>
+  </si>
+  <si>
+    <t>mutant_SO_129</t>
+  </si>
+  <si>
+    <t>mutant_SO_130</t>
+  </si>
+  <si>
+    <t>mutant_SO_131</t>
+  </si>
+  <si>
+    <t>mutant_SO_132</t>
+  </si>
+  <si>
+    <t>mutant_SO_133</t>
+  </si>
+  <si>
+    <t>mutant_SO_134</t>
+  </si>
+  <si>
+    <t>mutant_SO_135</t>
+  </si>
+  <si>
+    <t>mutant_SO_136</t>
+  </si>
+  <si>
+    <t>mutant_SO_137</t>
+  </si>
+  <si>
+    <t>mutant_SO_138</t>
+  </si>
+  <si>
+    <t>mutant_SO_139</t>
+  </si>
+  <si>
+    <t>mutant_SO_140</t>
+  </si>
+  <si>
+    <t>mutant_SO_141</t>
+  </si>
+  <si>
+    <t>mutant_SO_142</t>
+  </si>
+  <si>
+    <t>mutant_SO_143</t>
+  </si>
+  <si>
+    <t>mutant_SO_144</t>
+  </si>
+  <si>
+    <t>mutant_SO_145</t>
+  </si>
+  <si>
+    <t>mutant_SO_146</t>
+  </si>
+  <si>
+    <t>mutant_SO_147</t>
+  </si>
+  <si>
+    <t>mutant_SO_148</t>
+  </si>
+  <si>
+    <t>mutant_SO_149</t>
+  </si>
+  <si>
+    <t>mutant_SO_150</t>
+  </si>
+  <si>
+    <t>mutant_SO_151</t>
+  </si>
+  <si>
+    <t>mutant_SO_152</t>
+  </si>
+  <si>
+    <t>mutant_SO_153</t>
+  </si>
+  <si>
+    <t>mutant_SO_154</t>
+  </si>
+  <si>
+    <t>mutant_SO_155</t>
+  </si>
+  <si>
+    <t>mutant_SO_156</t>
+  </si>
+  <si>
+    <t>mutant_SO_157</t>
+  </si>
+  <si>
+    <t>mutant_SO_158</t>
+  </si>
+  <si>
+    <t>mutant_SO_159</t>
+  </si>
+  <si>
+    <t>mutant_SO_160</t>
+  </si>
+  <si>
+    <t>mutant_SO_161</t>
+  </si>
+  <si>
+    <t>mutant_SO_162</t>
+  </si>
+  <si>
+    <t>mutant_SO_163</t>
+  </si>
+  <si>
+    <t>mutant_SO_164</t>
+  </si>
+  <si>
+    <t>mutant_SO_166</t>
+  </si>
+  <si>
+    <t>mutant_SO_167</t>
+  </si>
+  <si>
+    <t>mutant_SO_168</t>
+  </si>
+  <si>
+    <t>mutant_SO_169</t>
+  </si>
+  <si>
+    <t>mutant_SO_170</t>
+  </si>
+  <si>
+    <t>mutant_SO_171</t>
+  </si>
+  <si>
+    <t>mutant_SO_172</t>
+  </si>
+  <si>
+    <t>mutant_SO_173</t>
+  </si>
+  <si>
+    <t>mutant_SO_174</t>
+  </si>
+  <si>
+    <t>mutant_SO_175</t>
+  </si>
+  <si>
+    <t>mutant_SO_176</t>
+  </si>
+  <si>
+    <t>mutant_SO_177</t>
+  </si>
+  <si>
+    <t>mutant_SO_178</t>
+  </si>
+  <si>
+    <t>mutant_SO_179</t>
+  </si>
+  <si>
+    <t>mutant_SO_180</t>
+  </si>
+  <si>
+    <t>mutant_SO_181</t>
+  </si>
+  <si>
+    <t>mutant_SO_182</t>
+  </si>
+  <si>
+    <t>mutant_SO_183</t>
+  </si>
+  <si>
+    <t>mutant_SO_184</t>
+  </si>
+  <si>
+    <t>mutant_SO_185</t>
+  </si>
+  <si>
+    <t>mutant_SO_186</t>
+  </si>
+  <si>
+    <t>mutant_SO_187</t>
+  </si>
+  <si>
+    <t>mutant_SO_188</t>
+  </si>
+  <si>
+    <t>mutant_SO_189</t>
+  </si>
+  <si>
+    <t>mutant_SO_190</t>
+  </si>
+  <si>
+    <t>Mutants</t>
   </si>
 </sst>
 </file>
@@ -653,7 +1302,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -718,6 +1367,13 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="I6" t="s">
+        <v>262</v>
+      </c>
+      <c r="J6">
+        <f>COUNTIF(B2:B38,"Done")</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -990,4 +1646,1279 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D03E70-7C1F-4D2C-A3CA-7793A2030B99}">
+  <dimension ref="A1:A252"/>
+  <sheetViews>
+    <sheetView topLeftCell="A235" workbookViewId="0">
+      <selection sqref="A1:A252"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- starting photography botium mutants
</commit_message>
<xml_diff>
--- a/mutation-analysis/mutants-rasa/results_photography.xlsx
+++ b/mutation-analysis/mutants-rasa/results_photography.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\satori\user-simulator-evaluation\mutation-analysis\mutants-rasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1FFBEC-D437-46D4-B0AE-4FFAEA84EB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9702217-941E-488B-A8B9-218110D7F8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="267">
   <si>
     <t>Sensei chat</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Survived</t>
   </si>
   <si>
-    <t>Killed ?</t>
-  </si>
-  <si>
     <t>El error es en las fechas parece casualidad</t>
   </si>
   <si>
@@ -838,21 +835,17 @@
   </si>
   <si>
     <t>Botium Mut. Score</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -891,7 +884,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -899,16 +892,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,79 +1325,103 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="F1" t="s">
-        <v>265</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="I6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J6">
         <f>COUNTIF(B2:B38,"Done")</f>
@@ -1394,276 +1429,412 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7">
+        <f>(COUNTIF(C2:C38,"Killed")+COUNTIF(D2:D38,"Killed"))/COUNTIF(B2:C38,"Done")</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7">
-        <f>COUNTIF(C2:C38,"Killed")/(COUNTIF(C2:C38,"Killed")+COUNTIF(C2:C38,"Survived"))</f>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="I9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J9">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="I10" t="s">
+        <v>265</v>
+      </c>
+      <c r="J10">
+        <f>COUNTIF(F2:F38,"Killed")/(COUNTIF(F2:F38,"Killed")+COUNTIF(F2:F38,"Survived"))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
+      <c r="C38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1692,1257 +1863,1257 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mutation analysis rasa & botium
</commit_message>
<xml_diff>
--- a/mutation-analysis/mutants-rasa/results_photography.xlsx
+++ b/mutation-analysis/mutants-rasa/results_photography.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\satori\user-simulator-evaluation\mutation-analysis\mutants-rasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9702217-941E-488B-A8B9-218110D7F8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DC580C-55C4-4F42-B0DF-41D0703D1346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="269">
   <si>
     <t>Sensei chat</t>
   </si>
@@ -838,6 +838,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>(timeout portfolio)</t>
+  </si>
+  <si>
+    <t>killed</t>
   </si>
 </sst>
 </file>
@@ -858,7 +864,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -883,8 +889,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -907,11 +931,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -920,6 +955,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,13 +1365,14 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1409,7 +1450,9 @@
       <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1457,7 +1500,9 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -1489,13 +1534,18 @@
         <v>4</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>267</v>
+      </c>
       <c r="I10" t="s">
         <v>265</v>
       </c>
       <c r="J10">
         <f>COUNTIF(F2:F38,"Killed")/(COUNTIF(F2:F38,"Killed")+COUNTIF(F2:F38,"Survived"))</f>
-        <v>0</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1519,18 +1569,20 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1553,20 +1605,22 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1582,9 +1636,12 @@
       <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1594,7 +1651,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1604,7 +1661,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -1618,23 +1675,27 @@
         <v>4</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1644,35 +1705,39 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="F23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1682,7 +1747,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1692,21 +1757,23 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1716,17 +1783,17 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1736,7 +1803,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1746,37 +1813,41 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -1799,18 +1870,20 @@
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -1823,18 +1896,20 @@
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>